<commit_message>
updated cost of emp docs
</commit_message>
<xml_diff>
--- a/raw_answers_github.xlsx
+++ b/raw_answers_github.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/BoorWiedmannLab/clm254_CarolineMotzer/Cost of EMP project/github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA59D53-4653-7B46-A6E5-3AED55BE7866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8B2CA8-BFC5-9847-BADD-BEDD90BF336C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56280" yWindow="3040" windowWidth="21240" windowHeight="24560" firstSheet="1" activeTab="1" xr2:uid="{DF039622-80E0-8746-8ADE-789E5DD4C210}"/>
+    <workbookView xWindow="58300" yWindow="1760" windowWidth="36780" windowHeight="21960" firstSheet="1" activeTab="1" xr2:uid="{DF039622-80E0-8746-8ADE-789E5DD4C210}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant identifier here" sheetId="1" r:id="rId1"/>
     <sheet name="raw_complete_results" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">raw_complete_results!$A$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">raw_complete_results!$A$1:$X$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="74">
   <si>
     <t>Question</t>
   </si>
@@ -171,9 +171,6 @@
     <t>lbs. milk solids processed annually</t>
   </si>
   <si>
-    <t>Had to call multiple times to get plant CP to respond</t>
-  </si>
-  <si>
     <t>Cheese</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>Plant identifier (Bolten et. al. 2024a;Bolten et. al. 2024b)</t>
   </si>
   <si>
-    <t>Commodity (Bolten et. al. 2024a;Bolten et. al. 2024b)</t>
-  </si>
-  <si>
     <t xml:space="preserve">7. After the 1‐year EMP project with Milk Quality Improvement Program, what would be the estimation of how much control you had over the pathogen presence in your processing environment? </t>
   </si>
   <si>
@@ -249,19 +243,25 @@
     <t>129/225 </t>
   </si>
   <si>
-    <t>Plant size (Bolten et. al. 2024a;b)</t>
-  </si>
-  <si>
-    <t># of swabs used (excluding swabs used by research team for initial sampling and final sampling and any investigational) (Bolten et. al. 2024a;b)</t>
-  </si>
-  <si>
-    <t>Mean prevalence (Bolten et. al. 2024a;b)</t>
-  </si>
-  <si>
-    <t>Initial sampling prevalence (Bolten et. al. 2024a;b)</t>
-  </si>
-  <si>
-    <t>Final sampling prevalence (Bolten et. al. 2024a;b)</t>
+    <t>Change in prevalence from initial sampling to final sampling</t>
+  </si>
+  <si>
+    <t>Plant size (Bolten et. al. 2024a;2024b)</t>
+  </si>
+  <si>
+    <t>Commodity (Bolten et. al. 2024a; 2024b)</t>
+  </si>
+  <si>
+    <t># of swabs used (excluding swabs used by research team for initial sampling and final sampling and any investigational) (Bolten et. al. 2024a;2024b)</t>
+  </si>
+  <si>
+    <t>overall prevalence (Bolten et. al. 2024a;2024b)</t>
+  </si>
+  <si>
+    <t>Initial sampling prevalence  (Bolten et. al. 2024a;2024b)</t>
+  </si>
+  <si>
+    <t>Follow-up sampling prevalence  (Bolten et. al. 2024a;2024b)</t>
   </si>
 </sst>
 </file>
@@ -846,11 +846,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAF3DD2-8476-7D4D-931C-8B87820EA32D}">
-  <dimension ref="A1:X29"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D33" sqref="D33"/>
+      <pane xSplit="2" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,41 +860,41 @@
     <col min="4" max="4" width="36.6640625" style="6" customWidth="1"/>
     <col min="5" max="6" width="16.5" style="6" customWidth="1"/>
     <col min="7" max="7" width="33.83203125" style="6" customWidth="1"/>
-    <col min="8" max="12" width="16.5" style="6" customWidth="1"/>
-    <col min="13" max="13" width="25.1640625" style="6" customWidth="1"/>
-    <col min="14" max="18" width="10.83203125" style="6"/>
-    <col min="19" max="19" width="51.1640625" style="6" customWidth="1"/>
-    <col min="20" max="20" width="44.1640625" style="6" customWidth="1"/>
-    <col min="21" max="21" width="31.1640625" style="6" customWidth="1"/>
-    <col min="22" max="22" width="25.6640625" style="6" customWidth="1"/>
-    <col min="23" max="23" width="21.6640625" style="6" customWidth="1"/>
-    <col min="24" max="16384" width="10.83203125" style="6"/>
+    <col min="8" max="13" width="16.5" style="6" customWidth="1"/>
+    <col min="14" max="14" width="25.1640625" style="6" customWidth="1"/>
+    <col min="15" max="19" width="10.83203125" style="6"/>
+    <col min="20" max="20" width="51.1640625" style="6" customWidth="1"/>
+    <col min="21" max="21" width="44.1640625" style="6" customWidth="1"/>
+    <col min="22" max="22" width="31.1640625" style="6" customWidth="1"/>
+    <col min="23" max="23" width="25.6640625" style="6" customWidth="1"/>
+    <col min="24" max="24" width="21.6640625" style="6" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>71</v>
@@ -906,51 +906,54 @@
         <v>73</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y1" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>39</v>
@@ -959,7 +962,7 @@
         <v>48100</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" s="13">
         <v>42</v>
@@ -976,52 +979,55 @@
       <c r="K2">
         <v>0.08</v>
       </c>
-      <c r="L2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="7">
+      <c r="L2">
+        <v>-42</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="7">
         <v>25000</v>
       </c>
-      <c r="N2" s="6">
+      <c r="O2" s="6">
         <v>0</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="P2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="Q2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="7">
         <v>10000</v>
       </c>
-      <c r="R2" s="7">
+      <c r="S2" s="7">
         <v>1200</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="T2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="U2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="14">
+      <c r="Y2" s="14">
         <v>25903</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>39</v>
@@ -1030,7 +1036,7 @@
         <v>156000</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G3" s="13">
         <v>10</v>
@@ -1047,52 +1053,55 @@
       <c r="K3">
         <v>0.25</v>
       </c>
-      <c r="L3" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="M3" s="7">
+      <c r="L3">
+        <v>-5</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="7">
         <v>2000</v>
       </c>
-      <c r="N3" s="6">
+      <c r="O3" s="6">
         <v>0</v>
       </c>
-      <c r="O3" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="P3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="7">
         <v>20000</v>
       </c>
-      <c r="R3" s="7">
+      <c r="S3" s="7">
         <v>5000</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="T3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="U3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="X3" s="15">
+      <c r="Y3" s="15">
         <v>2215</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>39</v>
@@ -1101,7 +1110,7 @@
         <v>390000</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" s="13">
         <v>37</v>
@@ -1118,47 +1127,50 @@
       <c r="K4">
         <v>0.03</v>
       </c>
-      <c r="L4" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="6">
+      <c r="O4" s="6">
         <v>2</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="R4" s="7">
         <v>100000</v>
       </c>
-      <c r="R4" s="7">
+      <c r="S4" s="7">
         <v>20000</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="T4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="U4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="V4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="W4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="X4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="14">
+      <c r="Y4" s="14">
         <v>5794.5</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
         <v>7</v>
@@ -1173,7 +1185,7 @@
         <v>35250</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G5" s="13">
         <v>10</v>
@@ -1190,47 +1202,50 @@
       <c r="K5">
         <v>0.15</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="M5" s="7">
+      <c r="L5">
+        <v>-48</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" s="7">
         <v>5000</v>
       </c>
-      <c r="N5" s="6">
+      <c r="O5" s="6">
         <v>0</v>
       </c>
-      <c r="O5" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="P5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="7">
         <v>100000</v>
       </c>
-      <c r="R5" s="7">
+      <c r="S5" s="7">
         <v>23000</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="T5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="U5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="V5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="W5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="X5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="X5" s="14">
+      <c r="Y5" s="14">
         <v>5215</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1244,7 +1259,7 @@
         <v>41125</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G6" s="13">
         <v>19</v>
@@ -1261,47 +1276,50 @@
       <c r="K6">
         <v>0.2</v>
       </c>
-      <c r="L6" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="6">
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="6">
         <v>980</v>
       </c>
-      <c r="N6" s="6">
+      <c r="O6" s="6">
         <v>0</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="P6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6" s="7">
         <v>7500</v>
       </c>
-      <c r="R6" s="7">
+      <c r="S6" s="7">
         <v>2000</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="T6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="U6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="V6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="W6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="W6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="X6" s="14">
+      <c r="X6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="14">
         <v>1388.5</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>40</v>
       </c>
@@ -1332,52 +1350,55 @@
       <c r="K7">
         <v>0.36</v>
       </c>
-      <c r="L7" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="M7" s="7">
+      <c r="L7">
+        <v>34</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="7">
         <v>5000</v>
       </c>
-      <c r="N7" s="6">
+      <c r="O7" s="6">
         <v>0</v>
       </c>
-      <c r="O7" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="P7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" s="9">
         <v>200000</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="S7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="S7" s="10" t="s">
+      <c r="T7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="U7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="U7" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="V7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="W7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="X7" s="14">
+      <c r="X7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y7" s="14">
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>39</v>
@@ -1386,7 +1407,7 @@
         <v>2600</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G8" s="13">
         <v>36</v>
@@ -1403,52 +1424,55 @@
       <c r="K8">
         <v>0.15</v>
       </c>
-      <c r="L8" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="M8" s="7">
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="N8" s="7">
         <v>400</v>
       </c>
-      <c r="N8" s="6">
+      <c r="O8" s="6">
         <v>0</v>
       </c>
-      <c r="O8" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="P8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" s="7">
         <v>40000</v>
       </c>
-      <c r="R8" s="7">
+      <c r="S8" s="7">
         <v>3000</v>
       </c>
-      <c r="S8" s="6" t="s">
+      <c r="T8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T8" s="6" t="s">
+      <c r="U8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="U8" s="6" t="s">
+      <c r="V8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V8" s="6" t="s">
+      <c r="W8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="W8" s="6" t="s">
+      <c r="X8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="X8" s="14">
+      <c r="Y8" s="14">
         <v>1186.96</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>38</v>
@@ -1457,7 +1481,7 @@
         <v>11050000</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G9" s="13">
         <v>562</v>
@@ -1474,52 +1498,55 @@
       <c r="K9">
         <v>0.06</v>
       </c>
-      <c r="L9" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="M9" s="7">
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" s="7">
         <v>200</v>
       </c>
-      <c r="N9" s="6">
+      <c r="O9" s="6">
         <v>0</v>
       </c>
-      <c r="O9" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="P9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="7">
         <v>2200000</v>
       </c>
-      <c r="R9" s="7">
+      <c r="S9" s="7">
         <v>250000</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="T9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="U9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="V9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="V9" s="6" t="s">
+      <c r="W9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="W9" s="6" t="s">
+      <c r="X9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="X9" s="14">
+      <c r="Y9" s="14">
         <v>12485.32</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>38</v>
@@ -1528,7 +1555,7 @@
         <v>1950000</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G10" s="12">
         <v>253</v>
@@ -1545,48 +1572,51 @@
       <c r="K10">
         <v>0.22</v>
       </c>
-      <c r="L10" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M10" s="7">
+      <c r="L10">
+        <v>-9</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10" s="7">
         <v>50000</v>
       </c>
-      <c r="N10" s="6">
+      <c r="O10" s="6">
         <v>0</v>
       </c>
-      <c r="O10" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="P10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="Q10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="7">
+      <c r="S10" s="7">
         <v>75000</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="T10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="U10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="V10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="V10" s="6" t="s">
+      <c r="W10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="W10" s="6" t="s">
+      <c r="X10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="X10" s="14">
+      <c r="Y10" s="14">
         <v>55530.58</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="Q15" s="8"/>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="R15" s="8"/>
     </row>
     <row r="27" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D27" s="11"/>
@@ -1598,19 +1628,19 @@
       <c r="D29" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W1" xr:uid="{ABAF3DD2-8476-7D4D-931C-8B87820EA32D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W10">
+  <autoFilter ref="A1:X1" xr:uid="{ABAF3DD2-8476-7D4D-931C-8B87820EA32D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X10">
       <sortCondition descending="1" ref="D1:D10"/>
     </sortState>
   </autoFilter>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576" xr:uid="{75737846-7E07-574E-ADAD-1E41F8DA8011}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W1048576" xr:uid="{75737846-7E07-574E-ADAD-1E41F8DA8011}">
       <formula1>"Not helpful at all, Moderately helpful, Helpful, Very helpful, Essential to success of our EMP"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576" xr:uid="{2EE9C191-F8AF-9C40-A44C-E36A213510A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576" xr:uid="{2EE9C191-F8AF-9C40-A44C-E36A213510A9}">
       <formula1>"No all need some consulting, Most need consulting, About half need consulting, Most don't need consulting, None need consulting"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576 S2:S9 S11:S1048576 D18:D26" xr:uid="{2A74E5E1-7D3F-BE43-80AB-1CD70A7C6CF3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576 T2:T9 T11:T1048576 D18:D26" xr:uid="{2A74E5E1-7D3F-BE43-80AB-1CD70A7C6CF3}">
       <formula1>"No control/No signs of improvement, Little control/Small signs of improvement, Some control/Some signs of improvement, Mostly under control/Obvious improvement, Full control/No improvements needed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>